<commit_message>
Implementing saving in existing file - ERROR DETECTED
</commit_message>
<xml_diff>
--- a/src/Files_Resource/Savings/intento1.xlsx
+++ b/src/Files_Resource/Savings/intento1.xlsx
@@ -12,7 +12,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
   <si>
     <t>Aggregate Capital Commitment</t>
   </si>
@@ -104,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -114,93 +120,93 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="n">
-        <v>5000000.0</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>3574319.0</v>
+        <v>5000000.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>4571832.0</v>
+        <v>3574319.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>5000000.0</v>
+        <v>4571832.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>-329257.0</v>
+        <v>5000000.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>-1844071.0</v>
+        <v>-329257.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>-4547648.0</v>
+        <v>-1844071.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>117218.0</v>
+        <v>-4547648.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>634519.0</v>
+        <v>117218.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>2909928.0</v>
+        <v>634519.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>3362280.0</v>
+        <v>2909928.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="n">
         <v>3362280.0</v>
@@ -208,7 +214,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="n">
         <v>3362280.0</v>
@@ -216,15 +222,15 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>2223231.0</v>
+        <v>3362280.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="n">
         <v>2223231.0</v>
@@ -232,9 +238,17 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="n">
+        <v>2223231.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="n">
         <v>2223231.0</v>
       </c>
     </row>

</xml_diff>